<commit_message>
Update templates, add questionnaire body and description
</commit_message>
<xml_diff>
--- a/src/main/resources/Template.xlsx
+++ b/src/main/resources/Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>[[question.qName]]</t>
   </si>
@@ -27,12 +27,18 @@
   <si>
     <t>[[question.note]]</t>
   </si>
+  <si>
+    <t>[[name]]</t>
+  </si>
+  <si>
+    <t>[[description]]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +73,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -96,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -119,24 +143,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="5"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="5" builtinId="17"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -440,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,36 +499,47 @@
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>